<commit_message>
add disk statistics scripts
</commit_message>
<xml_diff>
--- a/data/HSE各项综合信息月表_2025年2月.xlsx
+++ b/data/HSE各项综合信息月表_2025年2月.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_Work_Station\Work_Platform\A_Plan\Agent\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CE7668-2ACA-4998-A543-125526D95BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AF59996-3920-40F8-885A-FCA5D68EA858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{030F2A20-C7E3-4459-B6D2-71E2F4AD8D38}"/>
+    <workbookView xWindow="8565" yWindow="8340" windowWidth="20310" windowHeight="9135" xr2:uid="{7A5E0FB8-E478-46F0-92AE-0B3190159D0D}"/>
   </bookViews>
   <sheets>
-    <sheet name="费用统计" sheetId="5" r:id="rId1"/>
-    <sheet name="集群统计" sheetId="4" r:id="rId2"/>
-    <sheet name="slot使用情况统计" sheetId="3" r:id="rId3"/>
-    <sheet name="mem使用情况统计" sheetId="2" r:id="rId4"/>
-    <sheet name="队列统计" sheetId="1" r:id="rId5"/>
+    <sheet name="费用统计" sheetId="6" r:id="rId1"/>
+    <sheet name="集群统计" sheetId="5" r:id="rId2"/>
+    <sheet name="slot使用情况统计" sheetId="4" r:id="rId3"/>
+    <sheet name="mem使用情况统计" sheetId="3" r:id="rId4"/>
+    <sheet name="队列统计" sheetId="2" r:id="rId5"/>
+    <sheet name="磁盘统计" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="581">
   <si>
     <t>HSE团队名称</t>
   </si>
@@ -1072,6 +1073,708 @@
   </si>
   <si>
     <t>114 GiB</t>
+  </si>
+  <si>
+    <t>Funtion Leader</t>
+  </si>
+  <si>
+    <t>Domain Leader</t>
+  </si>
+  <si>
+    <t>Domain name</t>
+  </si>
+  <si>
+    <t>研发盘</t>
+  </si>
+  <si>
+    <t>备份盘</t>
+  </si>
+  <si>
+    <t>卷名</t>
+  </si>
+  <si>
+    <t>大小(T)</t>
+  </si>
+  <si>
+    <t>研发盘总量(T)</t>
+  </si>
+  <si>
+    <t>研发盘实际使用(T)</t>
+  </si>
+  <si>
+    <t>研发盘剩余(T)</t>
+  </si>
+  <si>
+    <t>研发盘总剩余(T)</t>
+  </si>
+  <si>
+    <t>大小（T）</t>
+  </si>
+  <si>
+    <t>备份盘总量(T)</t>
+  </si>
+  <si>
+    <t>5.0需求峰值</t>
+  </si>
+  <si>
+    <t>已分配</t>
+  </si>
+  <si>
+    <t>薛勃</t>
+  </si>
+  <si>
+    <t>IP_sip_dv</t>
+  </si>
+  <si>
+    <t>libra_IP_scratch_sipdv</t>
+  </si>
+  <si>
+    <t>projects_ci_sip</t>
+  </si>
+  <si>
+    <t>projects_ci_cdb_sip</t>
+  </si>
+  <si>
+    <t>李进</t>
+  </si>
+  <si>
+    <t>IP_processor</t>
+  </si>
+  <si>
+    <t>projects_ci_processor</t>
+  </si>
+  <si>
+    <t>邓良策</t>
+  </si>
+  <si>
+    <t>draco_IP_scratch_Interconnect</t>
+  </si>
+  <si>
+    <t>archive_IP_interconnect</t>
+  </si>
+  <si>
+    <t>draco_IP_scratch_aasp</t>
+  </si>
+  <si>
+    <t>IP_ccix</t>
+  </si>
+  <si>
+    <t>IP_aasp</t>
+  </si>
+  <si>
+    <t>IP_nebula</t>
+  </si>
+  <si>
+    <t>IP_pcie</t>
+  </si>
+  <si>
+    <t>projects_ci_interconnect</t>
+  </si>
+  <si>
+    <t>张鑫</t>
+  </si>
+  <si>
+    <t>socdv_sysipdv</t>
+  </si>
+  <si>
+    <t>archive_socdv</t>
+  </si>
+  <si>
+    <t>projects_ci_infra</t>
+  </si>
+  <si>
+    <t>projects_ci_socdv</t>
+  </si>
+  <si>
+    <t>projects_ci_sysip</t>
+  </si>
+  <si>
+    <t>socdv_socdv1</t>
+  </si>
+  <si>
+    <t>socdv_socdv2</t>
+  </si>
+  <si>
+    <t>socdv_infra</t>
+  </si>
+  <si>
+    <t>迟秀伟</t>
+  </si>
+  <si>
+    <t>projects_ci_cluster</t>
+  </si>
+  <si>
+    <t>IP_cluster</t>
+  </si>
+  <si>
+    <t>draco_IP_scratch_cluster</t>
+  </si>
+  <si>
+    <t>魏斌</t>
+  </si>
+  <si>
+    <t>perf_regr_sh</t>
+  </si>
+  <si>
+    <t>毕金琼</t>
+  </si>
+  <si>
+    <t>sysdv_sysdv_grp</t>
+  </si>
+  <si>
+    <t>projects_ci_sysdv</t>
+  </si>
+  <si>
+    <t>IP_common</t>
+  </si>
+  <si>
+    <t>何健彬</t>
+  </si>
+  <si>
+    <t>projects_ci_mc</t>
+  </si>
+  <si>
+    <t>李爽</t>
+  </si>
+  <si>
+    <t>projects_ci_dceip</t>
+  </si>
+  <si>
+    <t>archive_IP_dte</t>
+  </si>
+  <si>
+    <t>IP_scratch_dce</t>
+  </si>
+  <si>
+    <t>IP_dte</t>
+  </si>
+  <si>
+    <t>冯闯</t>
+  </si>
+  <si>
+    <t>draco_IP_scratch_sip_de</t>
+  </si>
+  <si>
+    <t>IP_despc</t>
+  </si>
+  <si>
+    <t>draco_IP_scratch_sip_de2</t>
+  </si>
+  <si>
+    <t>IP_benchmark</t>
+  </si>
+  <si>
+    <t>IP_sip</t>
+  </si>
+  <si>
+    <t>柴菁</t>
+  </si>
+  <si>
+    <t>吴飞</t>
+  </si>
+  <si>
+    <t>soc_design</t>
+  </si>
+  <si>
+    <t>IP_sysip</t>
+  </si>
+  <si>
+    <t>梁志坚</t>
+  </si>
+  <si>
+    <t>projects_ci_implip</t>
+  </si>
+  <si>
+    <t>孙立军</t>
+  </si>
+  <si>
+    <t>IP_fabric</t>
+  </si>
+  <si>
+    <t>耿红喜</t>
+  </si>
+  <si>
+    <t>NPE</t>
+  </si>
+  <si>
+    <t>archive_npe</t>
+  </si>
+  <si>
+    <t>IP_amos</t>
+  </si>
+  <si>
+    <t>尹鹏跃</t>
+  </si>
+  <si>
+    <t>马海英</t>
+  </si>
+  <si>
+    <t>郭锐</t>
+  </si>
+  <si>
+    <t>draco_dfx</t>
+  </si>
+  <si>
+    <t>archive_pavo_dfx</t>
+  </si>
+  <si>
+    <t>draco_dfx_dv</t>
+  </si>
+  <si>
+    <t>archive_scorpio_dfx</t>
+  </si>
+  <si>
+    <t>draco_dfx_mbist</t>
+  </si>
+  <si>
+    <t>pavo_DFX_SS</t>
+  </si>
+  <si>
+    <t>libra_dfx</t>
+  </si>
+  <si>
+    <t>archive_leo_dfx</t>
+  </si>
+  <si>
+    <t>libra_dfx_atpg_3</t>
+  </si>
+  <si>
+    <t>archive_venus_dft</t>
+  </si>
+  <si>
+    <t>scorpio_dfx_dv_soc</t>
+  </si>
+  <si>
+    <t>scorpio_dfx_atpg_2</t>
+  </si>
+  <si>
+    <t>scorpio_dfx_atpg_3</t>
+  </si>
+  <si>
+    <t>libra_dfx_dv_ip</t>
+  </si>
+  <si>
+    <t>libra_dfx_mbist</t>
+  </si>
+  <si>
+    <t>libra_dfx_atpg_1</t>
+  </si>
+  <si>
+    <t>draco_dfx_atpg_1</t>
+  </si>
+  <si>
+    <t>libra_dfx_atpg_2</t>
+  </si>
+  <si>
+    <t>libra_dfx_dv_soc</t>
+  </si>
+  <si>
+    <t>任承志</t>
+  </si>
+  <si>
+    <t>platform_new_platform1</t>
+  </si>
+  <si>
+    <t>archive_leo_Platform</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>殷妮</t>
+  </si>
+  <si>
+    <t>libra_impl_vclp</t>
+  </si>
+  <si>
+    <t>archive_leo_feint</t>
+  </si>
+  <si>
+    <t>soc_impl_ipa</t>
+  </si>
+  <si>
+    <t>archive_libra_impl</t>
+  </si>
+  <si>
+    <t>soc_impl_simulation</t>
+  </si>
+  <si>
+    <t>archive_soc_impl_FC</t>
+  </si>
+  <si>
+    <t>libra_impl_fclc</t>
+  </si>
+  <si>
+    <t>archive_dorado_FEINT</t>
+  </si>
+  <si>
+    <t>libra_impl_release</t>
+  </si>
+  <si>
+    <t>archive_leo_soc_impl</t>
+  </si>
+  <si>
+    <t>soc_impl</t>
+  </si>
+  <si>
+    <t>archive_pavo_soc_impl</t>
+  </si>
+  <si>
+    <t>soc_impl_FC</t>
+  </si>
+  <si>
+    <t>archive_scorpio_FEINT</t>
+  </si>
+  <si>
+    <t>soc_impl_IP</t>
+  </si>
+  <si>
+    <t>archive_xproj_dfx</t>
+  </si>
+  <si>
+    <t>draco_impl_fe_vol1</t>
+  </si>
+  <si>
+    <t>libra_impl_timing</t>
+  </si>
+  <si>
+    <t>libra_impl_syn</t>
+  </si>
+  <si>
+    <t>秦征</t>
+  </si>
+  <si>
+    <t>SIPI_LS_File</t>
+  </si>
+  <si>
+    <t>周建冲</t>
+  </si>
+  <si>
+    <t>analog_simulation</t>
+  </si>
+  <si>
+    <t>analog_design</t>
+  </si>
+  <si>
+    <t>东华</t>
+  </si>
+  <si>
+    <t>libra_pd_block3</t>
+  </si>
+  <si>
+    <t>archive_leo_ir_rhsc</t>
+  </si>
+  <si>
+    <t>libra_pd_block7</t>
+  </si>
+  <si>
+    <t>archive_leo_pd_a1</t>
+  </si>
+  <si>
+    <t>libra_pd_data</t>
+  </si>
+  <si>
+    <t>archive_leo_pd_a1sta</t>
+  </si>
+  <si>
+    <t>libra_pd_flow</t>
+  </si>
+  <si>
+    <t>archive_leo_spg</t>
+  </si>
+  <si>
+    <t>libra_pd_release</t>
+  </si>
+  <si>
+    <t>archive_libra_pd_block1</t>
+  </si>
+  <si>
+    <t>libra_pd_PHYV</t>
+  </si>
+  <si>
+    <t>archive_libra_pd_block1_folik</t>
+  </si>
+  <si>
+    <t>libra_pd_block_final_pr</t>
+  </si>
+  <si>
+    <t>archive_scorpio_folik_analog_design</t>
+  </si>
+  <si>
+    <t>libra_pd_FCPR</t>
+  </si>
+  <si>
+    <t>archive_scorpio_pd_FCT</t>
+  </si>
+  <si>
+    <t>efpd</t>
+  </si>
+  <si>
+    <t>libra_pd_block8</t>
+  </si>
+  <si>
+    <t>froot</t>
+  </si>
+  <si>
+    <t>pavo_PD</t>
+  </si>
+  <si>
+    <t>libra_pd_FCT</t>
+  </si>
+  <si>
+    <t>pd_report</t>
+  </si>
+  <si>
+    <t>libra_pd_block6</t>
+  </si>
+  <si>
+    <t>scorpio_pd_ESD</t>
+  </si>
+  <si>
+    <t>Ldidt</t>
+  </si>
+  <si>
+    <t>scorpio_pd_FCFP</t>
+  </si>
+  <si>
+    <t>libra_pd_Mem</t>
+  </si>
+  <si>
+    <t>scorpio_pd_FCPR</t>
+  </si>
+  <si>
+    <t>FSIR</t>
+  </si>
+  <si>
+    <t>scorpio_pd_FCT</t>
+  </si>
+  <si>
+    <t>libra_pd_SII</t>
+  </si>
+  <si>
+    <t>scorpio_pd_FSIR</t>
+  </si>
+  <si>
+    <t>libra_pd_block2</t>
+  </si>
+  <si>
+    <t>scorpio_pd_Mem</t>
+  </si>
+  <si>
+    <t>libra_pd_block4</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block1</t>
+  </si>
+  <si>
+    <t>draco_pd_block1</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block2</t>
+  </si>
+  <si>
+    <t>draco_pd_data</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block3</t>
+  </si>
+  <si>
+    <t>draco_pd_flow</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block4</t>
+  </si>
+  <si>
+    <t>libra_pd_IREM</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block5</t>
+  </si>
+  <si>
+    <t>libra_pd_block5</t>
+  </si>
+  <si>
+    <t>scorpio_pd_block6</t>
+  </si>
+  <si>
+    <t>libra_pd_FCFP</t>
+  </si>
+  <si>
+    <t>scorpio_pd_data</t>
+  </si>
+  <si>
+    <t>libra_pd_block1</t>
+  </si>
+  <si>
+    <t>scorpio_pd_flow</t>
+  </si>
+  <si>
+    <t>scorpio_pd_pinpoint</t>
+  </si>
+  <si>
+    <t>scorpio_pd_sipblk</t>
+  </si>
+  <si>
+    <t>scorpio_restrictedaccess_guc</t>
+  </si>
+  <si>
+    <t>archive_dorado_pd_PA</t>
+  </si>
+  <si>
+    <t>archive_leo_pd</t>
+  </si>
+  <si>
+    <t>archive_venus_PD_scratch_IREM</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_Block</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_Block_2</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_Cluster</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_FCFP</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_FCT</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_PhyV</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_data</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_interposer</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_pinpoint</t>
+  </si>
+  <si>
+    <t>archive_xproj_pd_release</t>
+  </si>
+  <si>
+    <t>pavo_PD_release</t>
+  </si>
+  <si>
+    <t>pavo_PD_scratch</t>
+  </si>
+  <si>
+    <t>pavo_data</t>
+  </si>
+  <si>
+    <t>scorpio_pd_PhyV</t>
+  </si>
+  <si>
+    <t>scorpio_pd_release</t>
+  </si>
+  <si>
+    <t>公共数据</t>
+  </si>
+  <si>
+    <t>磁盘位置</t>
+  </si>
+  <si>
+    <t>总大小（TB）</t>
+  </si>
+  <si>
+    <t>efnas_05_sas</t>
+  </si>
+  <si>
+    <t>common_DV</t>
+  </si>
+  <si>
+    <t>lab_CXMT</t>
+  </si>
+  <si>
+    <t>lab_GF65PKG</t>
+  </si>
+  <si>
+    <t>lab_SAMSUNG</t>
+  </si>
+  <si>
+    <t>lab_UMC65</t>
+  </si>
+  <si>
+    <t>lab_XMC</t>
+  </si>
+  <si>
+    <t>lab_dorado</t>
+  </si>
+  <si>
+    <t>lab_draco</t>
+  </si>
+  <si>
+    <t>lab_libra</t>
+  </si>
+  <si>
+    <t>lab_pavo</t>
+  </si>
+  <si>
+    <t>lab_scorpio</t>
+  </si>
+  <si>
+    <t>lab_xproj</t>
+  </si>
+  <si>
+    <t>efnas_05_sata</t>
+  </si>
+  <si>
+    <t>archive_lab_dorstar</t>
+  </si>
+  <si>
+    <t>archive_lab_pavo</t>
+  </si>
+  <si>
+    <t>archive_lab_scorpio</t>
+  </si>
+  <si>
+    <t>archive_lab_smic</t>
+  </si>
+  <si>
+    <t>lab_GF12LP</t>
+  </si>
+  <si>
+    <t>lab_GF12LPP</t>
+  </si>
+  <si>
+    <t>lab_T12FFC</t>
+  </si>
+  <si>
+    <t>efnas_07_sas</t>
+  </si>
+  <si>
+    <t>lab_TSMCN7</t>
+  </si>
+  <si>
+    <t>efnas_07_sata</t>
+  </si>
+  <si>
+    <t>archive_lab_TSMCN6</t>
+  </si>
+  <si>
+    <t>archive_lab_dorado</t>
+  </si>
+  <si>
+    <t>lab_GF14LPP</t>
+  </si>
+  <si>
+    <t>efnas_12_ssd_1</t>
+  </si>
+  <si>
+    <t>lab_proj</t>
+  </si>
+  <si>
+    <t>efnas_13_sas_1</t>
+  </si>
+  <si>
+    <t>lab_TSMCN6</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +2143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1615E38F-E2AE-47A7-B69D-EBBFD9BE8B59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A09F6-CB51-43F2-9BF9-CEF7A5237683}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1829,7 +2532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94102C1-FFB8-4644-A0E3-E5FE95715CA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDF45F5-740A-417C-85D7-92B96B9E194C}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1942,7 +2645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003EE443-B9EB-42EB-8BD4-2EF3D0F305D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5789C8-7807-4987-9212-551C329BB51B}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2606,7 +3309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953F07B6-2774-4ADE-9A97-FD1039E33008}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8FD85B-2D8D-4529-9E56-1F5540BBF1D6}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2920,7 +3623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427AD933-79AB-436D-919A-214D3D54C846}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994A785E-D0C0-45B1-BEA5-44A5ECB48903}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6588,4 +7291,2687 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A49147-E3D8-4CE4-996D-7897E77751A8}">
+  <dimension ref="A1:N152"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" t="s">
+        <v>350</v>
+      </c>
+      <c r="J1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H2" t="s">
+        <v>356</v>
+      </c>
+      <c r="I2" t="s">
+        <v>357</v>
+      </c>
+      <c r="J2" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" t="s">
+        <v>358</v>
+      </c>
+      <c r="L2" t="s">
+        <v>359</v>
+      </c>
+      <c r="M2" t="s">
+        <v>360</v>
+      </c>
+      <c r="N2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>15.5</v>
+      </c>
+      <c r="H3">
+        <v>3.5</v>
+      </c>
+      <c r="I3">
+        <v>9.8400000000000016</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E4">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>10.7</v>
+      </c>
+      <c r="H4">
+        <v>2.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>4.88</v>
+      </c>
+      <c r="H5">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.08</v>
+      </c>
+      <c r="H6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>368</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>6.96</v>
+      </c>
+      <c r="H7">
+        <v>3.04</v>
+      </c>
+      <c r="I7">
+        <v>4.6400000000000006</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>18</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>369</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>371</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>31</v>
+      </c>
+      <c r="G9">
+        <v>1.4</v>
+      </c>
+      <c r="H9">
+        <v>1.6</v>
+      </c>
+      <c r="I9">
+        <v>17.09</v>
+      </c>
+      <c r="J9" t="s">
+        <v>372</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>45</v>
+      </c>
+      <c r="N9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>2.4</v>
+      </c>
+      <c r="H10">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.3</v>
+      </c>
+      <c r="H11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>1.22</v>
+      </c>
+      <c r="H12">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>376</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>7.29</v>
+      </c>
+      <c r="H13">
+        <v>8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.8</v>
+      </c>
+      <c r="H14">
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <v>2.39</v>
+      </c>
+      <c r="H16">
+        <v>1.6099999999999999</v>
+      </c>
+      <c r="I16">
+        <v>25.09</v>
+      </c>
+      <c r="J16" t="s">
+        <v>381</v>
+      </c>
+      <c r="K16">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L16">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>382</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>0.09</v>
+      </c>
+      <c r="H17">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>383</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>0.5</v>
+      </c>
+      <c r="H18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>384</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1.17</v>
+      </c>
+      <c r="H19">
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>16.5</v>
+      </c>
+      <c r="H20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>386</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>5.26</v>
+      </c>
+      <c r="H21">
+        <v>14.74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>387</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>388</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>389</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>10.5</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
+        <v>1.7</v>
+      </c>
+      <c r="I23">
+        <v>5.4</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="N23">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>390</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>391</v>
+      </c>
+      <c r="E25">
+        <v>3.5</v>
+      </c>
+      <c r="G25">
+        <v>1.8</v>
+      </c>
+      <c r="H25">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>393</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>19.5</v>
+      </c>
+      <c r="G26">
+        <v>2.63</v>
+      </c>
+      <c r="H26">
+        <v>4.37</v>
+      </c>
+      <c r="I26">
+        <v>9.1000000000000014</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>28</v>
+      </c>
+      <c r="N26">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27">
+        <v>12.5</v>
+      </c>
+      <c r="G27">
+        <v>7.77</v>
+      </c>
+      <c r="H27">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>395</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+      <c r="G28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H28">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="I28">
+        <v>4.09</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>10</v>
+      </c>
+      <c r="N28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>0.7</v>
+      </c>
+      <c r="H29">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>397</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>4.01</v>
+      </c>
+      <c r="H30">
+        <v>0.99000000000000021</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>398</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>399</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>0.2</v>
+      </c>
+      <c r="H31">
+        <v>1.8</v>
+      </c>
+      <c r="I31">
+        <v>1.8</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>400</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>401</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>14</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32">
+        <v>1.9</v>
+      </c>
+      <c r="I32">
+        <v>3.73</v>
+      </c>
+      <c r="J32" t="s">
+        <v>402</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>403</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>404</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>6.67</v>
+      </c>
+      <c r="H34">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>405</v>
+      </c>
+      <c r="B35" t="s">
+        <v>405</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>406</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>48</v>
+      </c>
+      <c r="G35">
+        <v>7.69</v>
+      </c>
+      <c r="H35">
+        <v>5.31</v>
+      </c>
+      <c r="I35">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>44</v>
+      </c>
+      <c r="N35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>407</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>1.5</v>
+      </c>
+      <c r="H36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>408</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>3.41</v>
+      </c>
+      <c r="H37">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>409</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>410</v>
+      </c>
+      <c r="E39">
+        <v>20</v>
+      </c>
+      <c r="G39">
+        <v>15</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>411</v>
+      </c>
+      <c r="B40" t="s">
+        <v>412</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>413</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40">
+        <v>11</v>
+      </c>
+      <c r="G40">
+        <v>4.43</v>
+      </c>
+      <c r="H40">
+        <v>1.5700000000000003</v>
+      </c>
+      <c r="I40">
+        <v>3.99</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>414</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>2.58</v>
+      </c>
+      <c r="H41">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>415</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>416</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H42">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="I42">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>417</v>
+      </c>
+      <c r="C43" t="s">
+        <v>418</v>
+      </c>
+      <c r="D43" t="s">
+        <v>418</v>
+      </c>
+      <c r="E43">
+        <v>4.5</v>
+      </c>
+      <c r="F43">
+        <v>4.5</v>
+      </c>
+      <c r="G43">
+        <v>1.5</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>419</v>
+      </c>
+      <c r="C44" t="s">
+        <v>420</v>
+      </c>
+      <c r="D44" t="s">
+        <v>420</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>0.7</v>
+      </c>
+      <c r="H44">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I44">
+        <v>2.5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>421</v>
+      </c>
+      <c r="K44">
+        <v>0.5</v>
+      </c>
+      <c r="L44">
+        <v>0.5</v>
+      </c>
+      <c r="N44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>422</v>
+      </c>
+      <c r="D45" t="s">
+        <v>422</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>0.8</v>
+      </c>
+      <c r="H45">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>423</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>2.31</v>
+      </c>
+      <c r="H46">
+        <v>1.69</v>
+      </c>
+      <c r="I46">
+        <v>1.69</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>424</v>
+      </c>
+      <c r="B47" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>426</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>154</v>
+      </c>
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+      <c r="H47">
+        <v>3.5</v>
+      </c>
+      <c r="I47">
+        <v>62.84</v>
+      </c>
+      <c r="J47" t="s">
+        <v>427</v>
+      </c>
+      <c r="K47">
+        <v>4.7</v>
+      </c>
+      <c r="L47">
+        <v>17.2</v>
+      </c>
+      <c r="M47">
+        <v>126</v>
+      </c>
+      <c r="N47">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>1.46</v>
+      </c>
+      <c r="H48">
+        <v>0.54</v>
+      </c>
+      <c r="J48" t="s">
+        <v>429</v>
+      </c>
+      <c r="K48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>430</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>0.8</v>
+      </c>
+      <c r="H49">
+        <v>1.2</v>
+      </c>
+      <c r="J49" t="s">
+        <v>431</v>
+      </c>
+      <c r="K49">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>432</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <v>5.16</v>
+      </c>
+      <c r="H50">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="J50" t="s">
+        <v>433</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>434</v>
+      </c>
+      <c r="E51">
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>5.65</v>
+      </c>
+      <c r="H51">
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="J51" t="s">
+        <v>435</v>
+      </c>
+      <c r="K51">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>436</v>
+      </c>
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="G52">
+        <v>2.78</v>
+      </c>
+      <c r="H52">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>437</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="G53">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H53">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>438</v>
+      </c>
+      <c r="E54">
+        <v>8.5</v>
+      </c>
+      <c r="G54">
+        <v>3.37</v>
+      </c>
+      <c r="H54">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>439</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>0.3</v>
+      </c>
+      <c r="H55">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>440</v>
+      </c>
+      <c r="E56">
+        <v>12</v>
+      </c>
+      <c r="G56">
+        <v>7.16</v>
+      </c>
+      <c r="H56">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>441</v>
+      </c>
+      <c r="E57">
+        <v>34</v>
+      </c>
+      <c r="G57">
+        <v>27.7</v>
+      </c>
+      <c r="H57">
+        <v>6.3000000000000007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>442</v>
+      </c>
+      <c r="E58">
+        <v>8.5</v>
+      </c>
+      <c r="G58">
+        <v>5.91</v>
+      </c>
+      <c r="H58">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>443</v>
+      </c>
+      <c r="E59">
+        <v>35</v>
+      </c>
+      <c r="G59">
+        <v>15.3</v>
+      </c>
+      <c r="H59">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>444</v>
+      </c>
+      <c r="E60">
+        <v>14</v>
+      </c>
+      <c r="G60">
+        <v>10.8</v>
+      </c>
+      <c r="H60">
+        <v>3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>445</v>
+      </c>
+      <c r="B61" t="s">
+        <v>445</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>446</v>
+      </c>
+      <c r="E61">
+        <v>50</v>
+      </c>
+      <c r="F61">
+        <v>87</v>
+      </c>
+      <c r="G61">
+        <v>45.9</v>
+      </c>
+      <c r="H61">
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="I61">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="J61" t="s">
+        <v>447</v>
+      </c>
+      <c r="K61">
+        <v>1.2</v>
+      </c>
+      <c r="L61">
+        <v>1.2</v>
+      </c>
+      <c r="M61">
+        <v>97</v>
+      </c>
+      <c r="N61">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>448</v>
+      </c>
+      <c r="E62">
+        <v>37</v>
+      </c>
+      <c r="G62">
+        <v>20.9</v>
+      </c>
+      <c r="H62">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>411</v>
+      </c>
+      <c r="B63" t="s">
+        <v>449</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>450</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63">
+        <v>98</v>
+      </c>
+      <c r="G63">
+        <v>3.84</v>
+      </c>
+      <c r="H63">
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="I63">
+        <v>38.06</v>
+      </c>
+      <c r="J63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K63">
+        <v>0.8</v>
+      </c>
+      <c r="L63">
+        <v>93.3</v>
+      </c>
+      <c r="M63">
+        <v>58</v>
+      </c>
+      <c r="N63">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>452</v>
+      </c>
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="G64">
+        <v>5.44</v>
+      </c>
+      <c r="H64">
+        <v>1.5599999999999996</v>
+      </c>
+      <c r="J64" t="s">
+        <v>453</v>
+      </c>
+      <c r="K64">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>454</v>
+      </c>
+      <c r="E65">
+        <v>9</v>
+      </c>
+      <c r="G65">
+        <v>6.59</v>
+      </c>
+      <c r="H65">
+        <v>2.41</v>
+      </c>
+      <c r="J65" t="s">
+        <v>455</v>
+      </c>
+      <c r="K65">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>456</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="G66">
+        <v>4.33</v>
+      </c>
+      <c r="H66">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="J66" t="s">
+        <v>457</v>
+      </c>
+      <c r="K66">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>458</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>2.38</v>
+      </c>
+      <c r="H67">
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="J67" t="s">
+        <v>459</v>
+      </c>
+      <c r="K67">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>460</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>0.5</v>
+      </c>
+      <c r="H68">
+        <v>1.5</v>
+      </c>
+      <c r="J68" t="s">
+        <v>461</v>
+      </c>
+      <c r="K68">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>462</v>
+      </c>
+      <c r="E69">
+        <v>6</v>
+      </c>
+      <c r="G69">
+        <v>4.16</v>
+      </c>
+      <c r="H69">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="J69" t="s">
+        <v>463</v>
+      </c>
+      <c r="K69">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>464</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>0.7</v>
+      </c>
+      <c r="H70">
+        <v>1.3</v>
+      </c>
+      <c r="J70" t="s">
+        <v>465</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>466</v>
+      </c>
+      <c r="E71">
+        <v>25</v>
+      </c>
+      <c r="G71">
+        <v>0.7</v>
+      </c>
+      <c r="H71">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>467</v>
+      </c>
+      <c r="E72">
+        <v>9</v>
+      </c>
+      <c r="G72">
+        <v>8.6</v>
+      </c>
+      <c r="H72">
+        <v>0.40000000000000036</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>468</v>
+      </c>
+      <c r="E73">
+        <v>25</v>
+      </c>
+      <c r="G73">
+        <v>22.7</v>
+      </c>
+      <c r="H73">
+        <v>2.3000000000000007</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>469</v>
+      </c>
+      <c r="C74" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" t="s">
+        <v>310</v>
+      </c>
+      <c r="E74">
+        <v>12</v>
+      </c>
+      <c r="F74">
+        <v>12</v>
+      </c>
+      <c r="G74">
+        <v>7.81</v>
+      </c>
+      <c r="H74">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I74">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="J74" t="s">
+        <v>470</v>
+      </c>
+      <c r="K74">
+        <v>3</v>
+      </c>
+      <c r="L74">
+        <v>3</v>
+      </c>
+      <c r="M74">
+        <v>25</v>
+      </c>
+      <c r="N74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>471</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" t="s">
+        <v>472</v>
+      </c>
+      <c r="E75">
+        <v>6</v>
+      </c>
+      <c r="F75">
+        <v>8</v>
+      </c>
+      <c r="G75">
+        <v>3.9</v>
+      </c>
+      <c r="H75">
+        <v>2.1</v>
+      </c>
+      <c r="I75">
+        <v>3.3</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>8</v>
+      </c>
+      <c r="N75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>473</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="G76">
+        <v>0.8</v>
+      </c>
+      <c r="H76">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" t="s">
+        <v>474</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" t="s">
+        <v>475</v>
+      </c>
+      <c r="E77">
+        <v>20</v>
+      </c>
+      <c r="F77">
+        <v>338.29999999999995</v>
+      </c>
+      <c r="G77">
+        <v>14.1</v>
+      </c>
+      <c r="H77">
+        <v>5.9</v>
+      </c>
+      <c r="I77">
+        <v>81.97</v>
+      </c>
+      <c r="J77" t="s">
+        <v>476</v>
+      </c>
+      <c r="K77">
+        <v>4.7</v>
+      </c>
+      <c r="L77">
+        <v>139.82</v>
+      </c>
+      <c r="N77">
+        <v>346.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>477</v>
+      </c>
+      <c r="E78">
+        <v>16</v>
+      </c>
+      <c r="G78">
+        <v>10.5</v>
+      </c>
+      <c r="H78">
+        <v>5.5</v>
+      </c>
+      <c r="J78" t="s">
+        <v>478</v>
+      </c>
+      <c r="K78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>479</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="H79">
+        <v>0.49000000000000021</v>
+      </c>
+      <c r="J79" t="s">
+        <v>480</v>
+      </c>
+      <c r="K79">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>481</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>0.03</v>
+      </c>
+      <c r="H80">
+        <v>0.97</v>
+      </c>
+      <c r="J80" t="s">
+        <v>482</v>
+      </c>
+      <c r="K80">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>483</v>
+      </c>
+      <c r="E81">
+        <v>23</v>
+      </c>
+      <c r="G81">
+        <v>18</v>
+      </c>
+      <c r="H81">
+        <v>5</v>
+      </c>
+      <c r="J81" t="s">
+        <v>484</v>
+      </c>
+      <c r="K81">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>485</v>
+      </c>
+      <c r="E82">
+        <v>11</v>
+      </c>
+      <c r="G82">
+        <v>8.4</v>
+      </c>
+      <c r="H82">
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="J82" t="s">
+        <v>486</v>
+      </c>
+      <c r="K82">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>487</v>
+      </c>
+      <c r="E83">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>7.53</v>
+      </c>
+      <c r="H83">
+        <v>2.4699999999999998</v>
+      </c>
+      <c r="J83" t="s">
+        <v>488</v>
+      </c>
+      <c r="K83">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>489</v>
+      </c>
+      <c r="E84">
+        <v>6</v>
+      </c>
+      <c r="G84">
+        <v>4</v>
+      </c>
+      <c r="H84">
+        <v>2</v>
+      </c>
+      <c r="J84" t="s">
+        <v>490</v>
+      </c>
+      <c r="K84">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="85" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>491</v>
+      </c>
+      <c r="E85">
+        <v>16</v>
+      </c>
+      <c r="G85">
+        <v>11.4</v>
+      </c>
+      <c r="H85">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J85" t="s">
+        <v>492</v>
+      </c>
+      <c r="K85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>493</v>
+      </c>
+      <c r="E86">
+        <v>0.5</v>
+      </c>
+      <c r="G86">
+        <v>0.02</v>
+      </c>
+      <c r="H86">
+        <v>0.48</v>
+      </c>
+      <c r="J86" t="s">
+        <v>494</v>
+      </c>
+      <c r="K86">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="87" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>495</v>
+      </c>
+      <c r="E87">
+        <v>35</v>
+      </c>
+      <c r="G87">
+        <v>24.3</v>
+      </c>
+      <c r="H87">
+        <v>10.7</v>
+      </c>
+      <c r="J87" t="s">
+        <v>496</v>
+      </c>
+      <c r="K87">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="88" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>497</v>
+      </c>
+      <c r="E88">
+        <v>20</v>
+      </c>
+      <c r="G88">
+        <v>12.4</v>
+      </c>
+      <c r="H88">
+        <v>7.6</v>
+      </c>
+      <c r="J88" t="s">
+        <v>498</v>
+      </c>
+      <c r="K88">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="89" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>499</v>
+      </c>
+      <c r="E89">
+        <v>20</v>
+      </c>
+      <c r="G89">
+        <v>14.7</v>
+      </c>
+      <c r="H89">
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="J89" t="s">
+        <v>500</v>
+      </c>
+      <c r="K89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>501</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0.4</v>
+      </c>
+      <c r="H90">
+        <v>0.6</v>
+      </c>
+      <c r="J90" t="s">
+        <v>502</v>
+      </c>
+      <c r="K90">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>503</v>
+      </c>
+      <c r="E91">
+        <v>6.7</v>
+      </c>
+      <c r="G91">
+        <v>6.24</v>
+      </c>
+      <c r="H91">
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="J91" t="s">
+        <v>504</v>
+      </c>
+      <c r="K91">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>505</v>
+      </c>
+      <c r="E92">
+        <v>4</v>
+      </c>
+      <c r="G92">
+        <v>3.33</v>
+      </c>
+      <c r="H92">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="J92" t="s">
+        <v>506</v>
+      </c>
+      <c r="K92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>507</v>
+      </c>
+      <c r="E93">
+        <v>23</v>
+      </c>
+      <c r="G93">
+        <v>20.3</v>
+      </c>
+      <c r="H93">
+        <v>2.6999999999999993</v>
+      </c>
+      <c r="J93" t="s">
+        <v>508</v>
+      </c>
+      <c r="K93">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>509</v>
+      </c>
+      <c r="E94">
+        <v>31</v>
+      </c>
+      <c r="G94">
+        <v>27.2</v>
+      </c>
+      <c r="H94">
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="J94" t="s">
+        <v>510</v>
+      </c>
+      <c r="K94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>511</v>
+      </c>
+      <c r="E95">
+        <v>5</v>
+      </c>
+      <c r="G95">
+        <v>3.01</v>
+      </c>
+      <c r="H95">
+        <v>1.9900000000000002</v>
+      </c>
+      <c r="J95" t="s">
+        <v>512</v>
+      </c>
+      <c r="K95">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>513</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="G96">
+        <v>0.01</v>
+      </c>
+      <c r="H96">
+        <v>2.99</v>
+      </c>
+      <c r="J96" t="s">
+        <v>514</v>
+      </c>
+      <c r="K96">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="97" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>515</v>
+      </c>
+      <c r="E97">
+        <v>0.1</v>
+      </c>
+      <c r="G97">
+        <v>0.02</v>
+      </c>
+      <c r="H97">
+        <v>0.08</v>
+      </c>
+      <c r="J97" t="s">
+        <v>516</v>
+      </c>
+      <c r="K97">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="98" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>517</v>
+      </c>
+      <c r="E98">
+        <v>40</v>
+      </c>
+      <c r="G98">
+        <v>34</v>
+      </c>
+      <c r="H98">
+        <v>6</v>
+      </c>
+      <c r="J98" t="s">
+        <v>518</v>
+      </c>
+      <c r="K98">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="99" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>519</v>
+      </c>
+      <c r="E99">
+        <v>15</v>
+      </c>
+      <c r="G99">
+        <v>13.1</v>
+      </c>
+      <c r="H99">
+        <v>1.9000000000000004</v>
+      </c>
+      <c r="J99" t="s">
+        <v>520</v>
+      </c>
+      <c r="K99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>521</v>
+      </c>
+      <c r="E100">
+        <v>7</v>
+      </c>
+      <c r="G100">
+        <v>5.93</v>
+      </c>
+      <c r="H100">
+        <v>1.0700000000000003</v>
+      </c>
+      <c r="J100" t="s">
+        <v>522</v>
+      </c>
+      <c r="K100">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="101" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>523</v>
+      </c>
+      <c r="E101">
+        <v>21</v>
+      </c>
+      <c r="G101">
+        <v>14.9</v>
+      </c>
+      <c r="H101">
+        <v>6.1</v>
+      </c>
+      <c r="J101" t="s">
+        <v>524</v>
+      </c>
+      <c r="K101">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="102" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="J102" t="s">
+        <v>525</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="J103" t="s">
+        <v>526</v>
+      </c>
+      <c r="K103">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="104" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="J104" t="s">
+        <v>527</v>
+      </c>
+      <c r="K104">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="105" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="J105" t="s">
+        <v>528</v>
+      </c>
+      <c r="K105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="J106" t="s">
+        <v>529</v>
+      </c>
+      <c r="K106">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="107" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="J107" t="s">
+        <v>530</v>
+      </c>
+      <c r="K107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="J108" t="s">
+        <v>531</v>
+      </c>
+      <c r="K108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="J109" t="s">
+        <v>532</v>
+      </c>
+      <c r="K109">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="110" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="J110" t="s">
+        <v>533</v>
+      </c>
+      <c r="K110">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="111" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="J111" t="s">
+        <v>534</v>
+      </c>
+      <c r="K111">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="112" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="J112" t="s">
+        <v>535</v>
+      </c>
+      <c r="K112">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="J113" t="s">
+        <v>536</v>
+      </c>
+      <c r="K113">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="J114" t="s">
+        <v>537</v>
+      </c>
+      <c r="K114">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="J115" t="s">
+        <v>538</v>
+      </c>
+      <c r="K115">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="J116" t="s">
+        <v>539</v>
+      </c>
+      <c r="K116">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="J117" t="s">
+        <v>540</v>
+      </c>
+      <c r="K117">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="J118" t="s">
+        <v>541</v>
+      </c>
+      <c r="K118">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="J119" t="s">
+        <v>542</v>
+      </c>
+      <c r="K119">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="J120" t="s">
+        <v>543</v>
+      </c>
+      <c r="K120">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="J121" t="s">
+        <v>544</v>
+      </c>
+      <c r="K121">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="J122" t="s">
+        <v>545</v>
+      </c>
+      <c r="K122">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <v>963.80000000000007</v>
+      </c>
+      <c r="F123">
+        <v>963.8</v>
+      </c>
+      <c r="K123">
+        <v>267.21999999999991</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>547</v>
+      </c>
+      <c r="B126" t="s">
+        <v>352</v>
+      </c>
+      <c r="C126" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>549</v>
+      </c>
+      <c r="B127" t="s">
+        <v>550</v>
+      </c>
+      <c r="C127">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>549</v>
+      </c>
+      <c r="B128" t="s">
+        <v>551</v>
+      </c>
+      <c r="C128">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>549</v>
+      </c>
+      <c r="B129" t="s">
+        <v>552</v>
+      </c>
+      <c r="C129">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>549</v>
+      </c>
+      <c r="B130" t="s">
+        <v>553</v>
+      </c>
+      <c r="C130">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>549</v>
+      </c>
+      <c r="B131" t="s">
+        <v>554</v>
+      </c>
+      <c r="C131">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>549</v>
+      </c>
+      <c r="B132" t="s">
+        <v>555</v>
+      </c>
+      <c r="C132">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>549</v>
+      </c>
+      <c r="B133" t="s">
+        <v>556</v>
+      </c>
+      <c r="C133">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>549</v>
+      </c>
+      <c r="B134" t="s">
+        <v>557</v>
+      </c>
+      <c r="C134">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>549</v>
+      </c>
+      <c r="B135" t="s">
+        <v>558</v>
+      </c>
+      <c r="C135">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>549</v>
+      </c>
+      <c r="B136" t="s">
+        <v>559</v>
+      </c>
+      <c r="C136">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>549</v>
+      </c>
+      <c r="B137" t="s">
+        <v>560</v>
+      </c>
+      <c r="C137">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>549</v>
+      </c>
+      <c r="B138" t="s">
+        <v>561</v>
+      </c>
+      <c r="C138">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>562</v>
+      </c>
+      <c r="B139" t="s">
+        <v>563</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>562</v>
+      </c>
+      <c r="B140" t="s">
+        <v>564</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>562</v>
+      </c>
+      <c r="B141" t="s">
+        <v>565</v>
+      </c>
+      <c r="C141">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>562</v>
+      </c>
+      <c r="B142" t="s">
+        <v>566</v>
+      </c>
+      <c r="C142">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>562</v>
+      </c>
+      <c r="B143" t="s">
+        <v>567</v>
+      </c>
+      <c r="C143">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>562</v>
+      </c>
+      <c r="B144" t="s">
+        <v>568</v>
+      </c>
+      <c r="C144">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>562</v>
+      </c>
+      <c r="B145" t="s">
+        <v>569</v>
+      </c>
+      <c r="C145">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>570</v>
+      </c>
+      <c r="B146" t="s">
+        <v>571</v>
+      </c>
+      <c r="C146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>572</v>
+      </c>
+      <c r="B147" t="s">
+        <v>573</v>
+      </c>
+      <c r="C147">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>572</v>
+      </c>
+      <c r="B148" t="s">
+        <v>574</v>
+      </c>
+      <c r="C148">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>572</v>
+      </c>
+      <c r="B149" t="s">
+        <v>575</v>
+      </c>
+      <c r="C149">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>576</v>
+      </c>
+      <c r="B150" t="s">
+        <v>577</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>578</v>
+      </c>
+      <c r="B151" t="s">
+        <v>579</v>
+      </c>
+      <c r="C151">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>580</v>
+      </c>
+      <c r="C152">
+        <v>58.594999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>